<commit_message>
The proportion of algea was set from 0.33 to 0 for both "VKIGR" (Diatoms) and "ANTBL" (Cyanobacteria). No change of results is expected since the proportion refers to the overal chlorophyll-a content which was 0 all along.
</commit_message>
<xml_diff>
--- a/inst/extdata/misa_data/parameter_conversion.xlsx
+++ b/inst/extdata/misa_data/parameter_conversion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Desktop\server_austausch\R_interface\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\kwb.misa\inst\extdata\misa_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F9A48B-DC43-441F-84B3-0D5940BCE98E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9453DB0D-14B8-4E45-825D-DD07C6F637F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1170,7 +1170,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1516,7 +1516,7 @@
         <v>55</v>
       </c>
       <c r="D17">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
         <v>56</v>
@@ -1536,7 +1536,7 @@
         <v>58</v>
       </c>
       <c r="D18">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
         <v>59</v>

</xml_diff>